<commit_message>
add bucket with session
</commit_message>
<xml_diff>
--- a/Hamburger.xlsx
+++ b/Hamburger.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
   <si>
     <t>Repository</t>
   </si>
@@ -147,6 +147,12 @@
   </si>
   <si>
     <t>mock bucket as a map in app</t>
+  </si>
+  <si>
+    <t>Validation</t>
+  </si>
+  <si>
+    <t>Exceptions</t>
   </si>
 </sst>
 </file>
@@ -608,7 +614,7 @@
   <dimension ref="B2:P12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -750,8 +756,12 @@
         <v>7</v>
       </c>
       <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
+      <c r="F7" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>41</v>
+      </c>
       <c r="H7" s="5"/>
       <c r="I7" s="5" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
unit tests for bucket functionality
</commit_message>
<xml_diff>
--- a/Hamburger.xlsx
+++ b/Hamburger.xlsx
@@ -146,13 +146,13 @@
     <t>add application.properties file</t>
   </si>
   <si>
-    <t>mock bucket as a map in app</t>
-  </si>
-  <si>
     <t>Validation</t>
   </si>
   <si>
     <t>Exceptions</t>
+  </si>
+  <si>
+    <t>mock bucket as a list in app</t>
   </si>
 </sst>
 </file>
@@ -614,7 +614,7 @@
   <dimension ref="B2:P12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -702,7 +702,7 @@
         <v>31</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F5" s="5"/>
       <c r="G5" s="5" t="s">
@@ -757,10 +757,10 @@
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>41</v>
       </c>
       <c r="H7" s="5"/>
       <c r="I7" s="5" t="s">

</xml_diff>

<commit_message>
reimplemented receipt add new model
</commit_message>
<xml_diff>
--- a/Hamburger.xlsx
+++ b/Hamburger.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="41">
   <si>
     <t>Repository</t>
   </si>
@@ -147,6 +147,9 @@
   </si>
   <si>
     <t>Exceptions &amp; Validation</t>
+  </si>
+  <si>
+    <t>Promotion</t>
   </si>
 </sst>
 </file>
@@ -608,7 +611,7 @@
   <dimension ref="B2:P11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -706,7 +709,9 @@
       <c r="G5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="5"/>
+      <c r="H5" s="5" t="s">
+        <v>40</v>
+      </c>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
       <c r="K5" s="3"/>

</xml_diff>

<commit_message>
receipt, exceptions handler, date
</commit_message>
<xml_diff>
--- a/Hamburger.xlsx
+++ b/Hamburger.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="44">
   <si>
     <t>Repository</t>
   </si>
@@ -150,6 +150,15 @@
   </si>
   <si>
     <t>Promotion</t>
+  </si>
+  <si>
+    <t>add payment</t>
+  </si>
+  <si>
+    <t>deal with receipt number</t>
+  </si>
+  <si>
+    <t>STOCK!</t>
   </si>
 </sst>
 </file>
@@ -608,10 +617,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:P11"/>
+  <dimension ref="B2:P16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -883,6 +892,21 @@
       <c r="O11" s="3"/>
       <c r="P11" s="3"/>
     </row>
+    <row r="14" spans="2:16" ht="32" x14ac:dyDescent="0.2">
+      <c r="G14" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="G15" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="G16" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Changes in TDD plan
</commit_message>
<xml_diff>
--- a/Hamburger.xlsx
+++ b/Hamburger.xlsx
@@ -149,13 +149,13 @@
     <t>deal with receipt number</t>
   </si>
   <si>
-    <t>Promotion TDD</t>
-  </si>
-  <si>
     <t>8. Iteration</t>
   </si>
   <si>
     <t>add docker payment service</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Promotion </t>
   </si>
 </sst>
 </file>
@@ -617,7 +617,7 @@
   <dimension ref="B2:P14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -667,7 +667,7 @@
         <v>34</v>
       </c>
       <c r="K3" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
@@ -718,7 +718,7 @@
         <v>20</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
@@ -826,7 +826,7 @@
         <v>35</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K9" s="5" t="s">
         <v>27</v>

</xml_diff>